<commit_message>
Add demo with parameter-only population type
</commit_message>
<xml_diff>
--- a/atomica/library/combined_databook.xlsx
+++ b/atomica/library/combined_databook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{926983E6-7E17-4E42-91C9-711276D41F06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD5FF0F-8B5B-4A10-A546-09CABAA4877B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="52">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -184,6 +184,12 @@
   <si>
     <t>Aging UDT</t>
   </si>
+  <si>
+    <t>env</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
 </sst>
 </file>
 
@@ -232,7 +238,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -270,11 +276,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -293,6 +321,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2345,9 +2377,11 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2419,6 +2453,17 @@
       </c>
       <c r="C6" s="3" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -4374,8 +4419,8 @@
   </sheetPr>
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E29" sqref="E29:E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>